<commit_message>
added new ingredients and densities and aliases
</commit_message>
<xml_diff>
--- a/Ingredient_Table_Populated_Master 251105.xlsx
+++ b/Ingredient_Table_Populated_Master 251105.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dakshilkanakia/Downloads/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3AC63C-DB8A-DD41-A455-39AF9962B733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C439ADA-C267-334F-BE8F-11DE5852AA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12620" yWindow="780" windowWidth="21580" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6268" uniqueCount="2097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6270" uniqueCount="2099">
   <si>
     <t>ingredient_id</t>
   </si>
@@ -5941,9 +5941,6 @@
     <t>Medjool dates</t>
   </si>
   <si>
-    <t>dates medjool</t>
-  </si>
-  <si>
     <t>Clementines</t>
   </si>
   <si>
@@ -6289,9 +6286,6 @@
     <t>radishes;red radish;red radishes</t>
   </si>
   <si>
-    <t>mint leaves;fresh mint</t>
-  </si>
-  <si>
     <t>mung bean;mung bean sprout</t>
   </si>
   <si>
@@ -6314,6 +6308,18 @@
   </si>
   <si>
     <t>2025-11-09T21:23:37.567908</t>
+  </si>
+  <si>
+    <t>dates medjool; medjool date</t>
+  </si>
+  <si>
+    <t>mint leaves;fresh mint; mint leaf</t>
+  </si>
+  <si>
+    <t>lemon juice</t>
+  </si>
+  <si>
+    <t>dinosaur kale</t>
   </si>
 </sst>
 </file>
@@ -6689,9 +6695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A918" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I957" sqref="I957"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6796,7 +6802,7 @@
         <v>343</v>
       </c>
       <c r="C5" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="D5" t="s">
         <v>798</v>
@@ -7478,7 +7484,7 @@
         <v>375</v>
       </c>
       <c r="C37" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
       <c r="D37" t="s">
         <v>798</v>
@@ -7678,6 +7684,9 @@
       <c r="B46" t="s">
         <v>384</v>
       </c>
+      <c r="C46" t="s">
+        <v>2098</v>
+      </c>
       <c r="D46" t="s">
         <v>798</v>
       </c>
@@ -7741,6 +7750,9 @@
       <c r="B49" t="s">
         <v>387</v>
       </c>
+      <c r="C49" t="s">
+        <v>2097</v>
+      </c>
       <c r="D49" t="s">
         <v>798</v>
       </c>
@@ -8194,7 +8206,7 @@
         <v>408</v>
       </c>
       <c r="C71" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="D71" t="s">
         <v>798</v>
@@ -9999,7 +10011,7 @@
         <v>493</v>
       </c>
       <c r="C156" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="D156" t="s">
         <v>802</v>
@@ -10435,7 +10447,7 @@
         <v>513</v>
       </c>
       <c r="C176" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="D176" t="s">
         <v>803</v>
@@ -11635,7 +11647,7 @@
         <v>570</v>
       </c>
       <c r="C233" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="D233" t="s">
         <v>805</v>
@@ -11761,7 +11773,7 @@
         <v>245</v>
       </c>
       <c r="B239" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="C239" t="s">
         <v>760</v>
@@ -12416,7 +12428,7 @@
         <v>604</v>
       </c>
       <c r="C268" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="D268" t="s">
         <v>807</v>
@@ -14370,7 +14382,7 @@
         <v>905</v>
       </c>
       <c r="C360" t="s">
-        <v>2088</v>
+        <v>2096</v>
       </c>
       <c r="D360" t="s">
         <v>798</v>
@@ -15444,7 +15456,7 @@
         <v>1017</v>
       </c>
       <c r="C411" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="D411" t="s">
         <v>803</v>
@@ -21049,7 +21061,7 @@
         <v>1971</v>
       </c>
       <c r="C677" t="s">
-        <v>1972</v>
+        <v>2095</v>
       </c>
       <c r="D677" t="s">
         <v>798</v>
@@ -21092,10 +21104,10 @@
         <v>1515</v>
       </c>
       <c r="B679" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C679" t="s">
         <v>1973</v>
-      </c>
-      <c r="C679" t="s">
-        <v>1974</v>
       </c>
       <c r="D679" t="s">
         <v>798</v>
@@ -21138,10 +21150,10 @@
         <v>1517</v>
       </c>
       <c r="B681" t="s">
+        <v>1974</v>
+      </c>
+      <c r="C681" t="s">
         <v>1975</v>
-      </c>
-      <c r="C681" t="s">
-        <v>1976</v>
       </c>
       <c r="D681" t="s">
         <v>798</v>
@@ -21184,7 +21196,7 @@
         <v>1519</v>
       </c>
       <c r="B683" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="D683" t="s">
         <v>798</v>
@@ -21227,7 +21239,7 @@
         <v>1521</v>
       </c>
       <c r="B685" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="D685" t="s">
         <v>798</v>
@@ -21270,7 +21282,7 @@
         <v>1523</v>
       </c>
       <c r="B687" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="D687" t="s">
         <v>798</v>
@@ -21313,7 +21325,7 @@
         <v>1525</v>
       </c>
       <c r="B689" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="D689" t="s">
         <v>798</v>
@@ -21359,7 +21371,7 @@
         <v>1527</v>
       </c>
       <c r="B691" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="D691" t="s">
         <v>798</v>
@@ -21402,7 +21414,7 @@
         <v>1530</v>
       </c>
       <c r="B693" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="D693" t="s">
         <v>798</v>
@@ -21445,7 +21457,7 @@
         <v>1532</v>
       </c>
       <c r="B695" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="D695" t="s">
         <v>803</v>
@@ -21488,7 +21500,7 @@
         <v>1534</v>
       </c>
       <c r="B697" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="D697" t="s">
         <v>803</v>
@@ -21534,7 +21546,7 @@
         <v>1536</v>
       </c>
       <c r="B699" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="D699" t="s">
         <v>803</v>
@@ -21577,10 +21589,10 @@
         <v>1539</v>
       </c>
       <c r="B701" t="s">
+        <v>1985</v>
+      </c>
+      <c r="C701" t="s">
         <v>1986</v>
-      </c>
-      <c r="C701" t="s">
-        <v>1987</v>
       </c>
       <c r="D701" t="s">
         <v>803</v>
@@ -21623,7 +21635,7 @@
         <v>1541</v>
       </c>
       <c r="B703" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="D703" t="s">
         <v>803</v>
@@ -21666,10 +21678,10 @@
         <v>1543</v>
       </c>
       <c r="B705" t="s">
+        <v>1988</v>
+      </c>
+      <c r="C705" t="s">
         <v>1989</v>
-      </c>
-      <c r="C705" t="s">
-        <v>1990</v>
       </c>
       <c r="D705" t="s">
         <v>803</v>
@@ -21712,10 +21724,10 @@
         <v>1545</v>
       </c>
       <c r="B707" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C707" t="s">
         <v>1991</v>
-      </c>
-      <c r="C707" t="s">
-        <v>1992</v>
       </c>
       <c r="D707" t="s">
         <v>803</v>
@@ -21758,7 +21770,7 @@
         <v>1547</v>
       </c>
       <c r="B709" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="D709" t="s">
         <v>803</v>
@@ -21801,10 +21813,10 @@
         <v>1549</v>
       </c>
       <c r="B711" t="s">
+        <v>1993</v>
+      </c>
+      <c r="C711" t="s">
         <v>1994</v>
-      </c>
-      <c r="C711" t="s">
-        <v>1995</v>
       </c>
       <c r="D711" t="s">
         <v>803</v>
@@ -21847,7 +21859,7 @@
         <v>1551</v>
       </c>
       <c r="B713" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="D713" t="s">
         <v>803</v>
@@ -21890,7 +21902,7 @@
         <v>1553</v>
       </c>
       <c r="B715" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D715" t="s">
         <v>803</v>
@@ -21933,7 +21945,7 @@
         <v>1555</v>
       </c>
       <c r="B717" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="D717" t="s">
         <v>803</v>
@@ -21976,10 +21988,10 @@
         <v>1557</v>
       </c>
       <c r="B719" t="s">
+        <v>1998</v>
+      </c>
+      <c r="C719" t="s">
         <v>1999</v>
-      </c>
-      <c r="C719" t="s">
-        <v>2000</v>
       </c>
       <c r="D719" t="s">
         <v>803</v>
@@ -22022,7 +22034,7 @@
         <v>1559</v>
       </c>
       <c r="B721" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="D721" t="s">
         <v>803</v>
@@ -22065,7 +22077,7 @@
         <v>1561</v>
       </c>
       <c r="B723" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="D723" t="s">
         <v>803</v>
@@ -22108,7 +22120,7 @@
         <v>1563</v>
       </c>
       <c r="B725" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="D725" t="s">
         <v>803</v>
@@ -22151,7 +22163,7 @@
         <v>1565</v>
       </c>
       <c r="B727" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D727" t="s">
         <v>803</v>
@@ -22194,7 +22206,7 @@
         <v>1567</v>
       </c>
       <c r="B729" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="D729" t="s">
         <v>803</v>
@@ -22237,7 +22249,7 @@
         <v>1569</v>
       </c>
       <c r="B731" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D731" t="s">
         <v>803</v>
@@ -22280,7 +22292,7 @@
         <v>1571</v>
       </c>
       <c r="B733" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D733" t="s">
         <v>803</v>
@@ -22323,10 +22335,10 @@
         <v>1573</v>
       </c>
       <c r="B735" t="s">
+        <v>2007</v>
+      </c>
+      <c r="C735" t="s">
         <v>2008</v>
-      </c>
-      <c r="C735" t="s">
-        <v>2009</v>
       </c>
       <c r="D735" t="s">
         <v>803</v>
@@ -22369,7 +22381,7 @@
         <v>1575</v>
       </c>
       <c r="B737" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D737" t="s">
         <v>803</v>
@@ -22412,7 +22424,7 @@
         <v>1577</v>
       </c>
       <c r="B739" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D739" t="s">
         <v>803</v>
@@ -22455,7 +22467,7 @@
         <v>1579</v>
       </c>
       <c r="B741" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D741" t="s">
         <v>803</v>
@@ -22498,7 +22510,7 @@
         <v>1581</v>
       </c>
       <c r="B743" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D743" t="s">
         <v>803</v>
@@ -22541,7 +22553,7 @@
         <v>1583</v>
       </c>
       <c r="B745" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D745" t="s">
         <v>803</v>
@@ -22584,7 +22596,7 @@
         <v>1585</v>
       </c>
       <c r="B747" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D747" t="s">
         <v>803</v>
@@ -22627,7 +22639,7 @@
         <v>1587</v>
       </c>
       <c r="B749" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D749" t="s">
         <v>802</v>
@@ -22670,7 +22682,7 @@
         <v>1589</v>
       </c>
       <c r="B751" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D751" t="s">
         <v>802</v>
@@ -22713,7 +22725,7 @@
         <v>1591</v>
       </c>
       <c r="B753" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D753" t="s">
         <v>802</v>
@@ -22756,7 +22768,7 @@
         <v>1593</v>
       </c>
       <c r="B755" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D755" t="s">
         <v>802</v>
@@ -22799,7 +22811,7 @@
         <v>1595</v>
       </c>
       <c r="B757" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D757" t="s">
         <v>802</v>
@@ -22842,7 +22854,7 @@
         <v>1597</v>
       </c>
       <c r="B759" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D759" t="s">
         <v>802</v>
@@ -22885,7 +22897,7 @@
         <v>1599</v>
       </c>
       <c r="B761" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D761" t="s">
         <v>802</v>
@@ -22928,7 +22940,7 @@
         <v>1601</v>
       </c>
       <c r="B763" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D763" t="s">
         <v>802</v>
@@ -22971,7 +22983,7 @@
         <v>1603</v>
       </c>
       <c r="B765" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D765" t="s">
         <v>802</v>
@@ -23014,7 +23026,7 @@
         <v>1605</v>
       </c>
       <c r="B767" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D767" t="s">
         <v>802</v>
@@ -23057,7 +23069,7 @@
         <v>1607</v>
       </c>
       <c r="B769" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="D769" t="s">
         <v>802</v>
@@ -23100,7 +23112,7 @@
         <v>1609</v>
       </c>
       <c r="B771" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="D771" t="s">
         <v>802</v>
@@ -23143,7 +23155,7 @@
         <v>1611</v>
       </c>
       <c r="B773" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="D773" t="s">
         <v>802</v>
@@ -23186,7 +23198,7 @@
         <v>1613</v>
       </c>
       <c r="B775" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="D775" t="s">
         <v>802</v>
@@ -23229,7 +23241,7 @@
         <v>1615</v>
       </c>
       <c r="B777" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="D777" t="s">
         <v>802</v>
@@ -23272,7 +23284,7 @@
         <v>1617</v>
       </c>
       <c r="B779" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="D779" t="s">
         <v>802</v>
@@ -23315,10 +23327,10 @@
         <v>1619</v>
       </c>
       <c r="B781" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C781" t="s">
         <v>2032</v>
-      </c>
-      <c r="C781" t="s">
-        <v>2033</v>
       </c>
       <c r="D781" t="s">
         <v>802</v>
@@ -23361,7 +23373,7 @@
         <v>1621</v>
       </c>
       <c r="B783" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="D783" t="s">
         <v>802</v>
@@ -23407,7 +23419,7 @@
         <v>1623</v>
       </c>
       <c r="B785" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D785" t="s">
         <v>802</v>
@@ -23450,7 +23462,7 @@
         <v>1626</v>
       </c>
       <c r="B787" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D787" t="s">
         <v>801</v>
@@ -23493,10 +23505,10 @@
         <v>1628</v>
       </c>
       <c r="B789" t="s">
+        <v>2036</v>
+      </c>
+      <c r="C789" t="s">
         <v>2037</v>
-      </c>
-      <c r="C789" t="s">
-        <v>2038</v>
       </c>
       <c r="D789" t="s">
         <v>801</v>
@@ -23539,7 +23551,7 @@
         <v>1630</v>
       </c>
       <c r="B791" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="D791" t="s">
         <v>801</v>
@@ -23582,7 +23594,7 @@
         <v>1632</v>
       </c>
       <c r="B793" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="C793" t="s">
         <v>797</v>
@@ -23631,7 +23643,7 @@
         <v>1634</v>
       </c>
       <c r="B795" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="D795" t="s">
         <v>801</v>
@@ -23677,7 +23689,7 @@
         <v>1637</v>
       </c>
       <c r="B797" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="D797" t="s">
         <v>801</v>
@@ -23720,7 +23732,7 @@
         <v>1640</v>
       </c>
       <c r="B799" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="D799" t="s">
         <v>801</v>
@@ -23763,7 +23775,7 @@
         <v>1642</v>
       </c>
       <c r="B801" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="D801" t="s">
         <v>801</v>
@@ -23809,7 +23821,7 @@
         <v>1644</v>
       </c>
       <c r="B803" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="D803" t="s">
         <v>801</v>
@@ -23852,7 +23864,7 @@
         <v>1647</v>
       </c>
       <c r="B805" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="D805" t="s">
         <v>801</v>
@@ -23898,7 +23910,7 @@
         <v>1649</v>
       </c>
       <c r="B807" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="D807" t="s">
         <v>801</v>
@@ -23941,7 +23953,7 @@
         <v>1652</v>
       </c>
       <c r="B809" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="D809" t="s">
         <v>801</v>
@@ -23984,7 +23996,7 @@
         <v>1654</v>
       </c>
       <c r="B811" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="D811" t="s">
         <v>801</v>
@@ -24030,7 +24042,7 @@
         <v>1656</v>
       </c>
       <c r="B813" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="D813" t="s">
         <v>801</v>
@@ -24073,7 +24085,7 @@
         <v>1659</v>
       </c>
       <c r="B815" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="D815" t="s">
         <v>801</v>
@@ -24116,7 +24128,7 @@
         <v>1661</v>
       </c>
       <c r="B817" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="D817" t="s">
         <v>806</v>
@@ -24159,7 +24171,7 @@
         <v>1663</v>
       </c>
       <c r="B819" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="D819" t="s">
         <v>806</v>
@@ -24205,7 +24217,7 @@
         <v>1665</v>
       </c>
       <c r="B821" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="D821" t="s">
         <v>806</v>
@@ -24251,7 +24263,7 @@
         <v>1668</v>
       </c>
       <c r="B823" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="D823" t="s">
         <v>806</v>
@@ -24294,10 +24306,10 @@
         <v>1671</v>
       </c>
       <c r="B825" t="s">
+        <v>2055</v>
+      </c>
+      <c r="C825" t="s">
         <v>2056</v>
-      </c>
-      <c r="C825" t="s">
-        <v>2057</v>
       </c>
       <c r="D825" t="s">
         <v>806</v>
@@ -24340,7 +24352,7 @@
         <v>1673</v>
       </c>
       <c r="B827" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="D827" t="s">
         <v>806</v>
@@ -24383,7 +24395,7 @@
         <v>1675</v>
       </c>
       <c r="B829" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="D829" t="s">
         <v>806</v>
@@ -24426,7 +24438,7 @@
         <v>1677</v>
       </c>
       <c r="B831" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="D831" t="s">
         <v>806</v>
@@ -24469,7 +24481,7 @@
         <v>1679</v>
       </c>
       <c r="B833" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="D833" t="s">
         <v>806</v>
@@ -24512,7 +24524,7 @@
         <v>1681</v>
       </c>
       <c r="B835" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="D835" t="s">
         <v>806</v>
@@ -24555,7 +24567,7 @@
         <v>1683</v>
       </c>
       <c r="B837" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="D837" t="s">
         <v>804</v>
@@ -24598,7 +24610,7 @@
         <v>1685</v>
       </c>
       <c r="B839" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="D839" t="s">
         <v>804</v>
@@ -24641,10 +24653,10 @@
         <v>1687</v>
       </c>
       <c r="B841" t="s">
+        <v>2064</v>
+      </c>
+      <c r="C841" t="s">
         <v>2065</v>
-      </c>
-      <c r="C841" t="s">
-        <v>2066</v>
       </c>
       <c r="D841" t="s">
         <v>804</v>
@@ -24687,7 +24699,7 @@
         <v>1689</v>
       </c>
       <c r="B843" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D843" t="s">
         <v>804</v>
@@ -24730,7 +24742,7 @@
         <v>1691</v>
       </c>
       <c r="B845" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="D845" t="s">
         <v>804</v>
@@ -24773,7 +24785,7 @@
         <v>1693</v>
       </c>
       <c r="B847" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="D847" t="s">
         <v>804</v>
@@ -24816,7 +24828,7 @@
         <v>1695</v>
       </c>
       <c r="B849" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="D849" t="s">
         <v>804</v>
@@ -24859,7 +24871,7 @@
         <v>1697</v>
       </c>
       <c r="B851" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="D851" t="s">
         <v>804</v>
@@ -24902,7 +24914,7 @@
         <v>1699</v>
       </c>
       <c r="B853" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="D853" t="s">
         <v>801</v>
@@ -24911,13 +24923,13 @@
         <v>826</v>
       </c>
       <c r="F853" t="s">
+        <v>2072</v>
+      </c>
+      <c r="G853" t="s">
         <v>2073</v>
       </c>
-      <c r="G853" t="s">
-        <v>2074</v>
-      </c>
       <c r="H853" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="854" spans="1:8" x14ac:dyDescent="0.2">
@@ -24948,7 +24960,7 @@
         <v>1701</v>
       </c>
       <c r="B855" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="D855" t="s">
         <v>801</v>
@@ -24957,13 +24969,13 @@
         <v>826</v>
       </c>
       <c r="F855" t="s">
+        <v>2072</v>
+      </c>
+      <c r="G855" t="s">
         <v>2073</v>
       </c>
-      <c r="G855" t="s">
-        <v>2074</v>
-      </c>
       <c r="H855" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="856" spans="1:8" x14ac:dyDescent="0.2">
@@ -24994,7 +25006,7 @@
         <v>1703</v>
       </c>
       <c r="B857" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="D857" t="s">
         <v>806</v>
@@ -25003,13 +25015,13 @@
         <v>826</v>
       </c>
       <c r="F857" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="G857" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="H857" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="858" spans="1:8" x14ac:dyDescent="0.2">
@@ -27378,13 +27390,13 @@
     </row>
     <row r="960" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A960" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B960" t="s">
         <v>2078</v>
       </c>
-      <c r="B960" t="s">
+      <c r="C960" t="s">
         <v>2079</v>
-      </c>
-      <c r="C960" t="s">
-        <v>2080</v>
       </c>
       <c r="D960" t="s">
         <v>808</v>
@@ -27393,24 +27405,24 @@
         <v>823</v>
       </c>
       <c r="F960" t="s">
+        <v>2080</v>
+      </c>
+      <c r="G960" t="s">
         <v>2081</v>
       </c>
-      <c r="G960" t="s">
-        <v>2082</v>
-      </c>
       <c r="H960" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="961" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A961" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B961" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C961" t="s">
         <v>2093</v>
-      </c>
-      <c r="B961" t="s">
-        <v>2094</v>
-      </c>
-      <c r="C961" t="s">
-        <v>2095</v>
       </c>
       <c r="D961" t="s">
         <v>808</v>
@@ -27419,10 +27431,10 @@
         <v>819</v>
       </c>
       <c r="G961" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="H961" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>